<commit_message>
Amélioration dashboard : ajout des themes emploi, scolarisation, logement et résidences principales
</commit_message>
<xml_diff>
--- a/Data/Liste indicateurs statistiques/Agate - indicateurs statistiques_v2.xlsx
+++ b/Data/Liste indicateurs statistiques/Agate - indicateurs statistiques_v2.xlsx
@@ -15,10 +15,10 @@
     <sheet name="Zone predefinie" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">categorie!$A$1:$E$58</definedName>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">indicateur!$A$1:$D$229</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">categorie!$A$1:$D$58</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">indicateur!$B$1:$C$229</definedName>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">categorie!$A$1:$D$58</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">indicateur!$B$1:$C$229</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">categorie!$A$1:$E$58</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">indicateur!$A$1:$D$229</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">indicateur!$B$1:$D$229</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1449" uniqueCount="621">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1449" uniqueCount="625">
   <si>
     <t xml:space="preserve">domaine</t>
   </si>
@@ -1287,25 +1287,37 @@
     <t xml:space="preserve">a_scolarise2a5</t>
   </si>
   <si>
-    <t xml:space="preserve">Jeune scolarisé</t>
+    <t xml:space="preserve">Jeune scolarisé de 2 à 5 ans</t>
   </si>
   <si>
     <t xml:space="preserve">b_n_scolarise2a5</t>
   </si>
   <si>
-    <t xml:space="preserve">Jeune non scolarisé</t>
+    <t xml:space="preserve">Jeune non scolarisé de 2 à 5 ans</t>
   </si>
   <si>
     <t xml:space="preserve">a_scolarise6a15</t>
   </si>
   <si>
+    <t xml:space="preserve">Jeune scolarisé de 6 à 15 ans</t>
+  </si>
+  <si>
     <t xml:space="preserve">b_n_scolarise6a15</t>
   </si>
   <si>
+    <t xml:space="preserve">Jeune non scolarisé de 6 à 15 ans</t>
+  </si>
+  <si>
     <t xml:space="preserve">a_scolarise16a24</t>
   </si>
   <si>
+    <t xml:space="preserve">Jeune scolarisé de 16 à 24 ans</t>
+  </si>
+  <si>
     <t xml:space="preserve">b_n_scolarise16a24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jeune non scolarisé de 16 à 24 ans</t>
   </si>
   <si>
     <t xml:space="preserve">Résidence principale</t>
@@ -2259,7 +2271,7 @@
   <dimension ref="A1:K1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
+      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4215,7 +4227,7 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A1:E58"/>
+  <autoFilter ref="A1:D58"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -4234,8 +4246,8 @@
   </sheetPr>
   <dimension ref="A1:AMD1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C105" activeCellId="0" sqref="C105"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A97" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I109" activeCellId="0" sqref="I109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6801,7 +6813,7 @@
         <v>421</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
       <c r="E128" s="1" t="s">
         <v>211</v>
@@ -6818,10 +6830,10 @@
         <v>126</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="E129" s="1" t="s">
         <v>211</v>
@@ -6858,10 +6870,10 @@
         <v>131</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>418</v>
+        <v>426</v>
       </c>
       <c r="E131" s="1" t="s">
         <v>211</v>
@@ -6878,10 +6890,10 @@
         <v>131</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>420</v>
+        <v>428</v>
       </c>
       <c r="E132" s="1" t="s">
         <v>211</v>
@@ -7001,7 +7013,7 @@
         <v>62</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>425</v>
+        <v>429</v>
       </c>
       <c r="E138" s="1" t="s">
         <v>211</v>
@@ -7018,10 +7030,10 @@
         <v>61</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>426</v>
+        <v>430</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="E139" s="1" t="s">
         <v>211</v>
@@ -7038,10 +7050,10 @@
         <v>61</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>429</v>
+        <v>433</v>
       </c>
       <c r="E140" s="1" t="s">
         <v>211</v>
@@ -7058,10 +7070,10 @@
         <v>61</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>430</v>
+        <v>434</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>431</v>
+        <v>435</v>
       </c>
       <c r="E141" s="1" t="s">
         <v>211</v>
@@ -7078,10 +7090,10 @@
         <v>143</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>433</v>
+        <v>437</v>
       </c>
       <c r="E142" s="1" t="s">
         <v>211</v>
@@ -7098,10 +7110,10 @@
         <v>143</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>434</v>
+        <v>438</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>435</v>
+        <v>439</v>
       </c>
       <c r="E143" s="1" t="s">
         <v>211</v>
@@ -7118,10 +7130,10 @@
         <v>143</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>436</v>
+        <v>440</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>437</v>
+        <v>441</v>
       </c>
       <c r="E144" s="1" t="s">
         <v>211</v>
@@ -7138,10 +7150,10 @@
         <v>143</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>438</v>
+        <v>442</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
       <c r="E145" s="1" t="s">
         <v>211</v>
@@ -7158,10 +7170,10 @@
         <v>143</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>440</v>
+        <v>444</v>
       </c>
       <c r="D146" s="4" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
       <c r="E146" s="1" t="s">
         <v>211</v>
@@ -7178,10 +7190,10 @@
         <v>143</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>442</v>
+        <v>446</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>443</v>
+        <v>447</v>
       </c>
       <c r="E147" s="1" t="s">
         <v>211</v>
@@ -7198,10 +7210,10 @@
         <v>145</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="E148" s="1" t="s">
         <v>211</v>
@@ -7218,10 +7230,10 @@
         <v>145</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>447</v>
+        <v>451</v>
       </c>
       <c r="E149" s="1" t="s">
         <v>211</v>
@@ -7238,10 +7250,10 @@
         <v>145</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>448</v>
+        <v>452</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
       <c r="E150" s="1" t="s">
         <v>211</v>
@@ -7258,10 +7270,10 @@
         <v>145</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>450</v>
+        <v>454</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>451</v>
+        <v>455</v>
       </c>
       <c r="E151" s="1" t="s">
         <v>211</v>
@@ -7278,10 +7290,10 @@
         <v>148</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>452</v>
+        <v>456</v>
       </c>
       <c r="D152" s="4" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
       <c r="E152" s="1" t="s">
         <v>211</v>
@@ -7298,10 +7310,10 @@
         <v>148</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>454</v>
+        <v>458</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>455</v>
+        <v>459</v>
       </c>
       <c r="E153" s="1" t="s">
         <v>211</v>
@@ -7318,10 +7330,10 @@
         <v>148</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>456</v>
+        <v>460</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
       <c r="E154" s="1" t="s">
         <v>211</v>
@@ -7338,10 +7350,10 @@
         <v>148</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>458</v>
+        <v>462</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>459</v>
+        <v>463</v>
       </c>
       <c r="E155" s="1" t="s">
         <v>211</v>
@@ -7358,10 +7370,10 @@
         <v>148</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>460</v>
+        <v>464</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>461</v>
+        <v>465</v>
       </c>
       <c r="E156" s="1" t="s">
         <v>211</v>
@@ -7378,10 +7390,10 @@
         <v>150</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>462</v>
+        <v>466</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>463</v>
+        <v>467</v>
       </c>
       <c r="E157" s="1" t="s">
         <v>211</v>
@@ -7398,10 +7410,10 @@
         <v>150</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>464</v>
+        <v>468</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>465</v>
+        <v>469</v>
       </c>
       <c r="E158" s="1" t="s">
         <v>211</v>
@@ -7418,10 +7430,10 @@
         <v>150</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>466</v>
+        <v>470</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>467</v>
+        <v>471</v>
       </c>
       <c r="E159" s="1" t="s">
         <v>211</v>
@@ -7438,7 +7450,7 @@
         <v>153</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>468</v>
+        <v>472</v>
       </c>
       <c r="D160" s="1" t="s">
         <v>288</v>
@@ -7458,10 +7470,10 @@
         <v>153</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>469</v>
+        <v>473</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>470</v>
+        <v>474</v>
       </c>
       <c r="E161" s="1" t="s">
         <v>211</v>
@@ -7478,10 +7490,10 @@
         <v>153</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>471</v>
+        <v>475</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>472</v>
+        <v>476</v>
       </c>
       <c r="E162" s="1" t="s">
         <v>211</v>
@@ -7498,10 +7510,10 @@
         <v>153</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>473</v>
+        <v>477</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>474</v>
+        <v>478</v>
       </c>
       <c r="E163" s="1" t="s">
         <v>211</v>
@@ -7518,10 +7530,10 @@
         <v>153</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>475</v>
+        <v>479</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>476</v>
+        <v>480</v>
       </c>
       <c r="E164" s="1" t="s">
         <v>211</v>
@@ -7538,10 +7550,10 @@
         <v>156</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>477</v>
+        <v>481</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>478</v>
+        <v>482</v>
       </c>
       <c r="E165" s="1" t="s">
         <v>211</v>
@@ -7558,10 +7570,10 @@
         <v>156</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>479</v>
+        <v>483</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="E166" s="1" t="s">
         <v>211</v>
@@ -7578,10 +7590,10 @@
         <v>156</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>481</v>
+        <v>485</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>482</v>
+        <v>486</v>
       </c>
       <c r="E167" s="1" t="s">
         <v>211</v>
@@ -7598,10 +7610,10 @@
         <v>156</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>483</v>
+        <v>487</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>484</v>
+        <v>488</v>
       </c>
       <c r="E168" s="1" t="s">
         <v>211</v>
@@ -7618,10 +7630,10 @@
         <v>156</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>485</v>
+        <v>489</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
       <c r="E169" s="1" t="s">
         <v>211</v>
@@ -7638,10 +7650,10 @@
         <v>156</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>487</v>
+        <v>491</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>488</v>
+        <v>492</v>
       </c>
       <c r="E170" s="1" t="s">
         <v>211</v>
@@ -7658,10 +7670,10 @@
         <v>159</v>
       </c>
       <c r="C171" s="0" t="s">
-        <v>489</v>
+        <v>493</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>490</v>
+        <v>494</v>
       </c>
       <c r="E171" s="1" t="s">
         <v>211</v>
@@ -8690,10 +8702,10 @@
         <v>159</v>
       </c>
       <c r="C172" s="0" t="s">
-        <v>491</v>
+        <v>495</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>492</v>
+        <v>496</v>
       </c>
       <c r="E172" s="1" t="s">
         <v>211</v>
@@ -9722,10 +9734,10 @@
         <v>162</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>493</v>
+        <v>497</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>494</v>
+        <v>498</v>
       </c>
       <c r="E173" s="1" t="s">
         <v>211</v>
@@ -9742,10 +9754,10 @@
         <v>162</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>495</v>
+        <v>499</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>496</v>
+        <v>500</v>
       </c>
       <c r="E174" s="1" t="s">
         <v>211</v>
@@ -9782,10 +9794,10 @@
         <v>165</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="E176" s="1" t="s">
         <v>211</v>
@@ -9802,10 +9814,10 @@
         <v>165</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>447</v>
+        <v>451</v>
       </c>
       <c r="E177" s="1" t="s">
         <v>211</v>
@@ -9822,10 +9834,10 @@
         <v>165</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>448</v>
+        <v>452</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
       <c r="E178" s="1" t="s">
         <v>211</v>
@@ -9842,10 +9854,10 @@
         <v>165</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>450</v>
+        <v>454</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>451</v>
+        <v>455</v>
       </c>
       <c r="E179" s="1" t="s">
         <v>211</v>
@@ -9882,10 +9894,10 @@
         <v>167</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>452</v>
+        <v>456</v>
       </c>
       <c r="D181" s="2" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
       <c r="E181" s="1" t="s">
         <v>211</v>
@@ -9902,10 +9914,10 @@
         <v>167</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>454</v>
+        <v>458</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>455</v>
+        <v>459</v>
       </c>
       <c r="E182" s="1" t="s">
         <v>211</v>
@@ -9922,10 +9934,10 @@
         <v>167</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>456</v>
+        <v>460</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
       <c r="E183" s="1" t="s">
         <v>211</v>
@@ -9942,10 +9954,10 @@
         <v>167</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>458</v>
+        <v>462</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>459</v>
+        <v>463</v>
       </c>
       <c r="E184" s="1" t="s">
         <v>211</v>
@@ -9962,10 +9974,10 @@
         <v>167</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>460</v>
+        <v>464</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>461</v>
+        <v>465</v>
       </c>
       <c r="E185" s="1" t="s">
         <v>211</v>
@@ -9982,10 +9994,10 @@
         <v>169</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>462</v>
+        <v>466</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>463</v>
+        <v>467</v>
       </c>
       <c r="E186" s="1" t="s">
         <v>211</v>
@@ -10002,10 +10014,10 @@
         <v>169</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>464</v>
+        <v>468</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>465</v>
+        <v>469</v>
       </c>
       <c r="E187" s="1" t="s">
         <v>211</v>
@@ -10022,10 +10034,10 @@
         <v>169</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>466</v>
+        <v>470</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>467</v>
+        <v>471</v>
       </c>
       <c r="E188" s="1" t="s">
         <v>211</v>
@@ -10062,10 +10074,10 @@
         <v>171</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>477</v>
+        <v>481</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>478</v>
+        <v>482</v>
       </c>
       <c r="E190" s="1" t="s">
         <v>211</v>
@@ -10082,10 +10094,10 @@
         <v>171</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>479</v>
+        <v>483</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="E191" s="1" t="s">
         <v>211</v>
@@ -10102,10 +10114,10 @@
         <v>171</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>481</v>
+        <v>485</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>482</v>
+        <v>486</v>
       </c>
       <c r="E192" s="1" t="s">
         <v>211</v>
@@ -10122,10 +10134,10 @@
         <v>171</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>483</v>
+        <v>487</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>484</v>
+        <v>488</v>
       </c>
       <c r="E193" s="1" t="s">
         <v>211</v>
@@ -10142,10 +10154,10 @@
         <v>171</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>485</v>
+        <v>489</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
       <c r="E194" s="1" t="s">
         <v>211</v>
@@ -10162,10 +10174,10 @@
         <v>171</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>487</v>
+        <v>491</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>488</v>
+        <v>492</v>
       </c>
       <c r="E195" s="1" t="s">
         <v>211</v>
@@ -10202,10 +10214,10 @@
         <v>173</v>
       </c>
       <c r="C197" s="0" t="s">
-        <v>489</v>
+        <v>493</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>490</v>
+        <v>494</v>
       </c>
       <c r="E197" s="1" t="s">
         <v>211</v>
@@ -10222,10 +10234,10 @@
         <v>173</v>
       </c>
       <c r="C198" s="0" t="s">
-        <v>491</v>
+        <v>495</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>492</v>
+        <v>496</v>
       </c>
       <c r="E198" s="1" t="s">
         <v>211</v>
@@ -10262,10 +10274,10 @@
         <v>175</v>
       </c>
       <c r="C200" s="0" t="s">
-        <v>497</v>
+        <v>501</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>498</v>
+        <v>502</v>
       </c>
       <c r="E200" s="1" t="s">
         <v>211</v>
@@ -10282,10 +10294,10 @@
         <v>175</v>
       </c>
       <c r="C201" s="0" t="s">
-        <v>499</v>
+        <v>503</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>500</v>
+        <v>504</v>
       </c>
       <c r="E201" s="1" t="s">
         <v>211</v>
@@ -10302,10 +10314,10 @@
         <v>175</v>
       </c>
       <c r="C202" s="0" t="s">
-        <v>501</v>
+        <v>505</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>502</v>
+        <v>506</v>
       </c>
       <c r="E202" s="1" t="s">
         <v>211</v>
@@ -10342,10 +10354,10 @@
         <v>178</v>
       </c>
       <c r="C204" s="0" t="s">
-        <v>503</v>
+        <v>507</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>504</v>
+        <v>508</v>
       </c>
       <c r="E204" s="1" t="s">
         <v>211</v>
@@ -10362,10 +10374,10 @@
         <v>178</v>
       </c>
       <c r="C205" s="0" t="s">
-        <v>505</v>
+        <v>509</v>
       </c>
       <c r="D205" s="1" t="s">
-        <v>506</v>
+        <v>510</v>
       </c>
       <c r="E205" s="1" t="s">
         <v>211</v>
@@ -10402,10 +10414,10 @@
         <v>181</v>
       </c>
       <c r="C207" s="0" t="s">
-        <v>507</v>
+        <v>511</v>
       </c>
       <c r="D207" s="1" t="s">
-        <v>508</v>
+        <v>512</v>
       </c>
       <c r="E207" s="1" t="s">
         <v>211</v>
@@ -10422,10 +10434,10 @@
         <v>181</v>
       </c>
       <c r="C208" s="0" t="s">
-        <v>509</v>
+        <v>513</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>510</v>
+        <v>514</v>
       </c>
       <c r="E208" s="1" t="s">
         <v>211</v>
@@ -10462,10 +10474,10 @@
         <v>184</v>
       </c>
       <c r="C210" s="0" t="s">
-        <v>511</v>
+        <v>515</v>
       </c>
       <c r="D210" s="1" t="s">
-        <v>512</v>
+        <v>516</v>
       </c>
       <c r="E210" s="1" t="s">
         <v>211</v>
@@ -10482,10 +10494,10 @@
         <v>184</v>
       </c>
       <c r="C211" s="0" t="s">
-        <v>513</v>
+        <v>517</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>514</v>
+        <v>518</v>
       </c>
       <c r="E211" s="1" t="s">
         <v>211</v>
@@ -10522,10 +10534,10 @@
         <v>187</v>
       </c>
       <c r="C213" s="0" t="s">
-        <v>515</v>
+        <v>519</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>516</v>
+        <v>520</v>
       </c>
       <c r="E213" s="1" t="s">
         <v>211</v>
@@ -10542,10 +10554,10 @@
         <v>187</v>
       </c>
       <c r="C214" s="0" t="s">
-        <v>517</v>
+        <v>521</v>
       </c>
       <c r="D214" s="1" t="s">
-        <v>518</v>
+        <v>522</v>
       </c>
       <c r="E214" s="1" t="s">
         <v>211</v>
@@ -10582,10 +10594,10 @@
         <v>190</v>
       </c>
       <c r="C216" s="0" t="s">
-        <v>519</v>
+        <v>523</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>520</v>
+        <v>524</v>
       </c>
       <c r="E216" s="1" t="s">
         <v>211</v>
@@ -10602,10 +10614,10 @@
         <v>190</v>
       </c>
       <c r="C217" s="0" t="s">
-        <v>521</v>
+        <v>525</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>522</v>
+        <v>526</v>
       </c>
       <c r="E217" s="1" t="s">
         <v>211</v>
@@ -10622,10 +10634,10 @@
         <v>190</v>
       </c>
       <c r="C218" s="0" t="s">
-        <v>523</v>
+        <v>527</v>
       </c>
       <c r="D218" s="1" t="s">
-        <v>524</v>
+        <v>528</v>
       </c>
       <c r="E218" s="1" t="s">
         <v>211</v>
@@ -10642,10 +10654,10 @@
         <v>190</v>
       </c>
       <c r="C219" s="0" t="s">
-        <v>525</v>
+        <v>529</v>
       </c>
       <c r="D219" s="1" t="s">
-        <v>526</v>
+        <v>530</v>
       </c>
       <c r="E219" s="1" t="s">
         <v>211</v>
@@ -10682,10 +10694,10 @@
         <v>193</v>
       </c>
       <c r="C221" s="1" t="s">
-        <v>527</v>
+        <v>531</v>
       </c>
       <c r="D221" s="1" t="s">
-        <v>528</v>
+        <v>532</v>
       </c>
       <c r="E221" s="1" t="s">
         <v>211</v>
@@ -10702,10 +10714,10 @@
         <v>193</v>
       </c>
       <c r="C222" s="1" t="s">
-        <v>529</v>
+        <v>533</v>
       </c>
       <c r="D222" s="1" t="s">
-        <v>530</v>
+        <v>534</v>
       </c>
       <c r="E222" s="1" t="s">
         <v>211</v>
@@ -10742,10 +10754,10 @@
         <v>196</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>531</v>
+        <v>535</v>
       </c>
       <c r="D224" s="1" t="s">
-        <v>532</v>
+        <v>536</v>
       </c>
       <c r="E224" s="1" t="s">
         <v>211</v>
@@ -10762,10 +10774,10 @@
         <v>196</v>
       </c>
       <c r="C225" s="1" t="s">
-        <v>533</v>
+        <v>537</v>
       </c>
       <c r="D225" s="1" t="s">
-        <v>534</v>
+        <v>538</v>
       </c>
       <c r="E225" s="1" t="s">
         <v>211</v>
@@ -10802,10 +10814,10 @@
         <v>199</v>
       </c>
       <c r="C227" s="1" t="s">
-        <v>535</v>
+        <v>539</v>
       </c>
       <c r="D227" s="1" t="s">
-        <v>536</v>
+        <v>540</v>
       </c>
       <c r="E227" s="1" t="s">
         <v>211</v>
@@ -10822,10 +10834,10 @@
         <v>199</v>
       </c>
       <c r="C228" s="1" t="s">
-        <v>537</v>
+        <v>541</v>
       </c>
       <c r="D228" s="1" t="s">
-        <v>538</v>
+        <v>542</v>
       </c>
       <c r="E228" s="1" t="s">
         <v>211</v>
@@ -10874,7 +10886,7 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A1:D229"/>
+  <autoFilter ref="B1:C229"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -10905,18 +10917,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>539</v>
+        <v>543</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>540</v>
+        <v>544</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>541</v>
+        <v>545</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>542</v>
+        <v>546</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10924,15 +10936,15 @@
         <v>208</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>543</v>
+        <v>547</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>544</v>
+        <v>548</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>545</v>
+        <v>549</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10940,279 +10952,279 @@
         <v>211</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>546</v>
+        <v>550</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>547</v>
+        <v>551</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>548</v>
+        <v>552</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>549</v>
+        <v>553</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>550</v>
+        <v>554</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>551</v>
+        <v>555</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>552</v>
+        <v>556</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>553</v>
+        <v>557</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>554</v>
+        <v>558</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>555</v>
+        <v>559</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>556</v>
+        <v>560</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>557</v>
+        <v>561</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>558</v>
+        <v>562</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>559</v>
+        <v>563</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>560</v>
+        <v>564</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>561</v>
+        <v>565</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>562</v>
+        <v>566</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>563</v>
+        <v>567</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>564</v>
+        <v>568</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>565</v>
+        <v>569</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>566</v>
+        <v>570</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>567</v>
+        <v>571</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>568</v>
+        <v>572</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>569</v>
+        <v>573</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>570</v>
+        <v>574</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>571</v>
+        <v>575</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>572</v>
+        <v>576</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>573</v>
+        <v>577</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>574</v>
+        <v>578</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
-        <v>575</v>
+        <v>579</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>576</v>
+        <v>580</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>577</v>
+        <v>581</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>578</v>
+        <v>582</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
-        <v>579</v>
+        <v>583</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>580</v>
+        <v>584</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
-        <v>581</v>
+        <v>585</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>582</v>
+        <v>586</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
-        <v>583</v>
+        <v>587</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>584</v>
+        <v>588</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
-        <v>585</v>
+        <v>589</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>586</v>
+        <v>590</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
-        <v>587</v>
+        <v>591</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>588</v>
+        <v>592</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="s">
-        <v>589</v>
+        <v>593</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>590</v>
+        <v>594</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
-        <v>591</v>
+        <v>595</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>592</v>
+        <v>596</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5" t="s">
-        <v>593</v>
+        <v>597</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="s">
-        <v>595</v>
+        <v>599</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>596</v>
+        <v>600</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="5" t="s">
-        <v>597</v>
+        <v>601</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>598</v>
+        <v>602</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>599</v>
+        <v>603</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>600</v>
+        <v>604</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>601</v>
+        <v>605</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>602</v>
+        <v>606</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>603</v>
+        <v>607</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>604</v>
+        <v>608</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="5" t="s">
-        <v>605</v>
+        <v>609</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>606</v>
+        <v>610</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="5" t="s">
-        <v>607</v>
+        <v>611</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>608</v>
+        <v>612</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="5" t="s">
-        <v>609</v>
+        <v>613</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>610</v>
+        <v>614</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="5" t="s">
-        <v>611</v>
+        <v>615</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>612</v>
+        <v>616</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>613</v>
+        <v>617</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>614</v>
+        <v>618</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -11245,10 +11257,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>615</v>
+        <v>619</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>616</v>
+        <v>620</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11256,7 +11268,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>617</v>
+        <v>621</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11264,7 +11276,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>618</v>
+        <v>622</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11272,7 +11284,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>619</v>
+        <v>623</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11280,7 +11292,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>620</v>
+        <v>624</v>
       </c>
     </row>
   </sheetData>

</xml_diff>